<commit_message>
Updated model comparison to include survreg
</commit_message>
<xml_diff>
--- a/ModelComparison.xlsx
+++ b/ModelComparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Bootstrap Independent</t>
   </si>
@@ -177,6 +177,24 @@
   </si>
   <si>
     <t>median from LN 7.8(1.8, 11.7)</t>
+  </si>
+  <si>
+    <t>Survreg</t>
+  </si>
+  <si>
+    <t>6.0 (4.7, 8.0)</t>
+  </si>
+  <si>
+    <t>2.5 (passed in to get it to fit)</t>
+  </si>
+  <si>
+    <t>12.15 (7.9, 18.6)</t>
+  </si>
+  <si>
+    <t>10.3 (7.0,15.4)</t>
+  </si>
+  <si>
+    <t>3.8 (passed in to get fit)</t>
   </si>
 </sst>
 </file>
@@ -508,7 +526,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,6 +535,7 @@
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -529,11 +548,17 @@
       <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -548,6 +573,9 @@
       <c r="D3" t="s">
         <v>44</v>
       </c>
+      <c r="E3">
+        <v>1.35</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -576,6 +604,9 @@
       <c r="D5" t="s">
         <v>41</v>
       </c>
+      <c r="E5">
+        <v>3.7</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -590,6 +621,9 @@
       <c r="D6" t="s">
         <v>42</v>
       </c>
+      <c r="E6">
+        <v>10.1</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -608,6 +642,9 @@
       <c r="D8" t="s">
         <v>50</v>
       </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -619,6 +656,9 @@
       <c r="D9" t="s">
         <v>49</v>
       </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
@@ -632,6 +672,9 @@
       <c r="D10" t="s">
         <v>46</v>
       </c>
+      <c r="E10">
+        <v>2.7</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -643,6 +686,9 @@
       <c r="D11" t="s">
         <v>47</v>
       </c>
+      <c r="E11">
+        <v>10.5</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -654,6 +700,9 @@
       <c r="D12" t="s">
         <v>48</v>
       </c>
+      <c r="E12">
+        <v>18.8</v>
+      </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -675,6 +724,9 @@
       <c r="D14" t="s">
         <v>38</v>
       </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -689,6 +741,9 @@
       <c r="D15" t="s">
         <v>39</v>
       </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -703,6 +758,9 @@
       <c r="D16" t="s">
         <v>40</v>
       </c>
+      <c r="E16">
+        <v>4.7</v>
+      </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -718,6 +776,9 @@
       <c r="D17" t="s">
         <v>36</v>
       </c>
+      <c r="E17">
+        <v>9.4</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -732,6 +793,9 @@
       <c r="D18" t="s">
         <v>37</v>
       </c>
+      <c r="E18">
+        <v>13.8</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G20" s="2"/>
@@ -748,5 +812,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated comparison sheet based on latest data update.
</commit_message>
<xml_diff>
--- a/ModelComparison.xlsx
+++ b/ModelComparison.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Bootstrap Independent</t>
   </si>
@@ -77,124 +80,79 @@
     <t>Serocooverison</t>
   </si>
   <si>
-    <t>12.7 (10.496-22.047)</t>
-  </si>
-  <si>
-    <t>10.1 (8.7-13.2)</t>
-  </si>
-  <si>
-    <t>6.7 (4.5-11.9)</t>
-  </si>
-  <si>
-    <t>6.4 (3.0-236)</t>
-  </si>
-  <si>
-    <t>10.7 (9.2-14.1)</t>
-  </si>
-  <si>
-    <t>10.0 (8.0-12.6)</t>
-  </si>
-  <si>
-    <t>3.8 (1.8-4.0)</t>
-  </si>
-  <si>
-    <t>3.9 (1.9-5.4)</t>
-  </si>
-  <si>
-    <t>8.9 (7.0-11.1)</t>
-  </si>
-  <si>
-    <t>14.3 (11.2-22.3)</t>
-  </si>
-  <si>
-    <t>10.6 (7.2-14.9)</t>
-  </si>
-  <si>
-    <t>2.5 (0.9-3.9)</t>
-  </si>
-  <si>
-    <t>3.1 (0.39-5.4)</t>
-  </si>
-  <si>
-    <t>9.0 (5.5-12.3)</t>
-  </si>
-  <si>
-    <t>18.2 (12.2-36.7)</t>
-  </si>
-  <si>
-    <t>3.2 (1.7-4.6)</t>
-  </si>
-  <si>
-    <t>11.8 (7.7-20.6)</t>
-  </si>
-  <si>
-    <t>6.0 (4.6, 7.8)</t>
-  </si>
-  <si>
-    <t>1.48 (1.22-2.01)</t>
-  </si>
-  <si>
-    <t>9.0 (7.1,11.1)</t>
-  </si>
-  <si>
-    <t>12.2 (8.9-23.6)</t>
-  </si>
-  <si>
-    <t>median from LN 9.0, (7.0,11.1)</t>
-  </si>
-  <si>
-    <t>dispersion from LN 1.20 (1.02,1.8)</t>
-  </si>
-  <si>
-    <t>6.9 (2.9, 8.7)</t>
-  </si>
-  <si>
-    <t>3.0 (1.5-4.4)</t>
-  </si>
-  <si>
-    <t>10.7 (7.5-21.2)</t>
-  </si>
-  <si>
-    <t>JAGS LLL</t>
-  </si>
-  <si>
-    <t>5.7 (4.3, 7.5)</t>
-  </si>
-  <si>
-    <t>1.47 (1.2, 2.1)</t>
-  </si>
-  <si>
-    <t>2.6 (0.03, 7.3)</t>
-  </si>
-  <si>
-    <t>7.8 (1.8, 11.7)</t>
-  </si>
-  <si>
-    <t>22.2 (12.0, 213.9)</t>
-  </si>
-  <si>
-    <t>dispersion form LN  1.9 (1.2, 12.8)</t>
-  </si>
-  <si>
-    <t>median from LN 7.8(1.8, 11.7)</t>
-  </si>
-  <si>
     <t>Survreg</t>
   </si>
   <si>
-    <t>6.0 (4.7, 8.0)</t>
-  </si>
-  <si>
-    <t>2.5 (passed in to get it to fit)</t>
-  </si>
-  <si>
-    <t>12.15 (7.9, 18.6)</t>
-  </si>
-  <si>
-    <t>10.3 (7.0,15.4)</t>
-  </si>
-  <si>
-    <t>3.8 (passed in to get fit)</t>
+    <t>6.4 (3.0-235)</t>
+  </si>
+  <si>
+    <t>10.7 (9.3-14.2)</t>
+  </si>
+  <si>
+    <t>6.8 (4.5-11.9)</t>
+  </si>
+  <si>
+    <t>10.1 (8.8-13.3)</t>
+  </si>
+  <si>
+    <t>12.7 (10.4-19.4)</t>
+  </si>
+  <si>
+    <t>3.2 (1.8-4.6)</t>
+  </si>
+  <si>
+    <t>11.2 (7.8-17.8)</t>
+  </si>
+  <si>
+    <t>5.9 (4.6, 7.5)</t>
+  </si>
+  <si>
+    <t>1.45 (1.23, 1.91)</t>
+  </si>
+  <si>
+    <t>2.7 (1.2-3.9)</t>
+  </si>
+  <si>
+    <t>3.4 (2.0-4.0)</t>
+  </si>
+  <si>
+    <t>10.1 (7.9-12.7)</t>
+  </si>
+  <si>
+    <t>3.5 (0.84-5.6)</t>
+  </si>
+  <si>
+    <t>11.1 (8.2-14.8)</t>
+  </si>
+  <si>
+    <t>9.5 (6.5-12.6)</t>
+  </si>
+  <si>
+    <t>17.9 (12.4-32.9)</t>
+  </si>
+  <si>
+    <t>4.0 (2.1-5.5)</t>
+  </si>
+  <si>
+    <t>8.9 (7.0-11.3)</t>
+  </si>
+  <si>
+    <t>14.3 (11.1, 19.2)</t>
+  </si>
+  <si>
+    <t>6.2 (4.7, 8.0)</t>
+  </si>
+  <si>
+    <t>12.4 (8.3,18.6)</t>
+  </si>
+  <si>
+    <t>2.7 (passed in to get it to fit)</t>
+  </si>
+  <si>
+    <t>3.4 (passed in to get fit)</t>
+  </si>
+  <si>
+    <t>10.5 (7.0,15.8)</t>
   </si>
 </sst>
 </file>
@@ -247,8 +205,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -523,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,11 +520,10 @@
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,21 +531,15 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -568,16 +547,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -585,13 +561,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -599,16 +575,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5">
+        <v>23</v>
+      </c>
+      <c r="D5">
         <v>3.7</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -616,199 +589,166 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6">
-        <v>10.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" t="s">
-        <v>53</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12">
-        <v>18.8</v>
-      </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="D12">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16">
-        <v>4.7</v>
-      </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17">
+        <v>35</v>
+      </c>
+      <c r="D17">
         <v>9.4</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18">
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="D18">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E24" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Model comparison chart updated with LWW JAGS model results
</commit_message>
<xml_diff>
--- a/ModelComparison.xlsx
+++ b/ModelComparison.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Bootstrap Independent</t>
   </si>
@@ -153,6 +153,51 @@
   </si>
   <si>
     <t>10.5 (7.0,15.8)</t>
+  </si>
+  <si>
+    <t>JAGS LWW</t>
+  </si>
+  <si>
+    <t>3.5 (1.5-7.2)</t>
+  </si>
+  <si>
+    <t>10.0 (7.8-12.9)</t>
+  </si>
+  <si>
+    <t>4.3(1.3-7.0)</t>
+  </si>
+  <si>
+    <t>9.0 (6.5-11.4)</t>
+  </si>
+  <si>
+    <t>13.8 (10.6-21.9)</t>
+  </si>
+  <si>
+    <t>10.9 (7.2-18.6)</t>
+  </si>
+  <si>
+    <t>2.0 (0.6-4.5)</t>
+  </si>
+  <si>
+    <t>2.4 (0.1-5.9)</t>
+  </si>
+  <si>
+    <t>9.1 (4.8-13.3)</t>
+  </si>
+  <si>
+    <t>19.0 (12.7-89.8)</t>
+  </si>
+  <si>
+    <t>5.0 (4.4, 7.7)</t>
+  </si>
+  <si>
+    <t>1.4 (1.22,2.0)</t>
+  </si>
+  <si>
+    <t>3.2 (1.6, 4.6)</t>
+  </si>
+  <si>
+    <t>10.7 (7.6-19.8)</t>
   </si>
 </sst>
 </file>
@@ -509,18 +554,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -533,6 +579,9 @@
       <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -552,6 +601,9 @@
       <c r="D3" t="s">
         <v>37</v>
       </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -566,6 +618,9 @@
       <c r="D4">
         <v>1.35</v>
       </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -580,6 +635,9 @@
       <c r="D5">
         <v>3.7</v>
       </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -594,6 +652,9 @@
       <c r="D6">
         <v>10</v>
       </c>
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -612,6 +673,9 @@
       <c r="D8" t="s">
         <v>38</v>
       </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -623,6 +687,9 @@
       <c r="D9" t="s">
         <v>39</v>
       </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
@@ -636,6 +703,9 @@
       <c r="D10">
         <v>4.0999999999999996</v>
       </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -647,6 +717,9 @@
       <c r="D11">
         <v>10.8</v>
       </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -658,6 +731,9 @@
       <c r="D12">
         <v>18.600000000000001</v>
       </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -679,6 +755,11 @@
       <c r="D14" t="s">
         <v>41</v>
       </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -693,6 +774,9 @@
       <c r="D15" t="s">
         <v>40</v>
       </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -707,9 +791,12 @@
       <c r="D16">
         <v>4.4000000000000004</v>
       </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -722,8 +809,12 @@
       <c r="D17">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -736,19 +827,39 @@
       <c r="D18">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="3"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated and finalized Rmd file to produce the supplement, including sensitivity analyses.
</commit_message>
<xml_diff>
--- a/ModelComparison.xlsx
+++ b/ModelComparison.xlsx
@@ -557,7 +557,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,6 +587,7 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -601,7 +602,7 @@
       <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -618,7 +619,7 @@
       <c r="D4">
         <v>1.35</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -635,7 +636,7 @@
       <c r="D5">
         <v>3.7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>55</v>
       </c>
     </row>
@@ -652,7 +653,7 @@
       <c r="D6">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -660,6 +661,7 @@
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E7" s="1"/>
       <c r="L7" s="2"/>
       <c r="N7" s="2"/>
     </row>
@@ -673,7 +675,7 @@
       <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -687,7 +689,7 @@
       <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>49</v>
       </c>
       <c r="J9" s="2"/>
@@ -703,7 +705,7 @@
       <c r="D10">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -717,7 +719,7 @@
       <c r="D11">
         <v>10.8</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -731,7 +733,7 @@
       <c r="D12">
         <v>18.600000000000001</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>52</v>
       </c>
       <c r="H12" s="3"/>
@@ -740,6 +742,7 @@
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E13" s="1"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -755,7 +758,7 @@
       <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>44</v>
       </c>
       <c r="K14" s="2"/>
@@ -774,7 +777,7 @@
       <c r="D15" t="s">
         <v>40</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -791,7 +794,7 @@
       <c r="D16">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H16" s="3"/>
@@ -809,7 +812,7 @@
       <c r="D17">
         <v>9.4</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I17" s="3"/>
@@ -827,7 +830,7 @@
       <c r="D18">
         <v>14.5</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>47</v>
       </c>
       <c r="I18" s="3"/>

</xml_diff>

<commit_message>
Some model comparison changes were not uploaded.
</commit_message>
<xml_diff>
--- a/ModelComparison.xlsx
+++ b/ModelComparison.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>Bootstrap Independent</t>
   </si>
@@ -198,6 +198,39 @@
   </si>
   <si>
     <t>10.7 (7.6-19.8)</t>
+  </si>
+  <si>
+    <t>Jags LLL</t>
+  </si>
+  <si>
+    <t>5.6 (4.4,7.2)</t>
+  </si>
+  <si>
+    <t>1.44 (1.22, 1.9)</t>
+  </si>
+  <si>
+    <t>3.2 (1.7, 4.5)</t>
+  </si>
+  <si>
+    <t>10.5(7.3, 16.9)</t>
+  </si>
+  <si>
+    <t>3.9 (0.1,7.7)</t>
+  </si>
+  <si>
+    <t>8.5 (3.8,12)</t>
+  </si>
+  <si>
+    <t>33.4(12,592)</t>
+  </si>
+  <si>
+    <t>6.9 (3.6, 8.8)</t>
+  </si>
+  <si>
+    <t>9.0 (7.4, 10.1)</t>
+  </si>
+  <si>
+    <t>12.4 (8.9,19.5)</t>
   </si>
 </sst>
 </file>
@@ -557,7 +590,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +615,9 @@
       <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -605,6 +641,9 @@
       <c r="E3" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -622,6 +661,9 @@
       <c r="E4" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -639,6 +681,9 @@
       <c r="E5" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -656,6 +701,9 @@
       <c r="E6" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -708,6 +756,9 @@
       <c r="E10" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -722,6 +773,9 @@
       <c r="E11" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -736,6 +790,9 @@
       <c r="E12" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -797,6 +854,9 @@
       <c r="E16" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="F16" t="s">
+        <v>65</v>
+      </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -815,6 +875,9 @@
       <c r="E17" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="F17" t="s">
+        <v>66</v>
+      </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -832,6 +895,9 @@
       </c>
       <c r="E18" s="1" t="s">
         <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>67</v>
       </c>
       <c r="I18" s="3"/>
     </row>

</xml_diff>